<commit_message>
update xpath for accounts payable
</commit_message>
<xml_diff>
--- a/BaswareAutomation/Output/OutputDataProvide.xlsx
+++ b/BaswareAutomation/Output/OutputDataProvide.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaswareAutomation\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\BaswareAutomation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -107,9 +107,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>EXON</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>S00011626001</t>
   </si>
   <si>
-    <t>Inv-C119/1/StdPO/1</t>
-  </si>
-  <si>
     <t>NatureCode</t>
   </si>
   <si>
@@ -149,10 +143,16 @@
     <t>Invoice</t>
   </si>
   <si>
-    <t>Test Status</t>
-  </si>
-  <si>
-    <t>FAIL</t>
+    <t>Test119/1</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>D200E</t>
   </si>
 </sst>
 </file>
@@ -179,22 +179,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -248,9 +238,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -267,7 +254,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -549,35 +541,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C3" sqref="A3:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="6" width="11.85546875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="21.140625" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="8" width="26.28515625" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="24.42578125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.140625" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="11.140625" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.85546875" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="17.42578125" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
-    <col min="20" max="20" style="1" width="9.140625" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="false"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.85546875" collapsed="false"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" width="10.28515625" collapsed="false"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="6"/>
+    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="1"/>
+    <col min="21" max="21" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -593,14 +587,14 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -623,7 +617,7 @@
       <c r="N1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -642,7 +636,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>13</v>
@@ -659,91 +653,85 @@
       <c r="Z1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="Q2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="12" t="s">
+      <c r="T2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="10">
-        <v>30</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="10">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s" s="19">
-        <v>42</v>
+      <c r="Y2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Approval List Exception updated and SSP wait solution
</commit_message>
<xml_diff>
--- a/BaswareAutomation/Output/OutputDataProvide.xlsx
+++ b/BaswareAutomation/Output/OutputDataProvide.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -32,7 +32,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -41,7 +41,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 A - Agency
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -74,6 +74,12 @@
     <t>Delivery Address</t>
   </si>
   <si>
+    <t>Approver2</t>
+  </si>
+  <si>
+    <t>Approver3</t>
+  </si>
+  <si>
     <t>PR tYPE</t>
   </si>
   <si>
@@ -107,121 +113,103 @@
     <t>Requestor</t>
   </si>
   <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>Provide2018</t>
+  </si>
+  <si>
+    <t>EMEAAD\igrabe</t>
+  </si>
+  <si>
     <t>Invoicing Address</t>
   </si>
   <si>
-    <t>Architect</t>
-  </si>
-  <si>
-    <t>RealEstateReference</t>
+    <t>Description PR1</t>
+  </si>
+  <si>
+    <t>Product 1</t>
+  </si>
+  <si>
+    <t>Guarding and security Event</t>
+  </si>
+  <si>
+    <t>S00000912001</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>30JDF</t>
+  </si>
+  <si>
+    <t>CS-FVAR</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Bruxelles Triomphe</t>
+  </si>
+  <si>
+    <t>Sopra Steria Benelux SA/NV</t>
+  </si>
+  <si>
+    <t>EMEAAD\hdehalleux</t>
+  </si>
+  <si>
+    <t>EMEAAD\aanciaux</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>https://voflusoprasttest.p2p.basware.com/edge</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2564</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>362</t>
+  </si>
+  <si>
+    <t>PRForm</t>
+  </si>
+  <si>
+    <t>STANDARD</t>
   </si>
   <si>
     <t>Agency/Site</t>
   </si>
   <si>
-    <t>Provide2018</t>
+    <t>0643</t>
   </si>
   <si>
     <t>Approver1</t>
   </si>
   <si>
-    <t>https://voflusoprasttest.p2p.basware.com</t>
-  </si>
-  <si>
-    <t>ProductCode</t>
-  </si>
-  <si>
-    <t>SSP</t>
-  </si>
-  <si>
-    <t>Product1</t>
-  </si>
-  <si>
-    <t>Approver2</t>
-  </si>
-  <si>
-    <t>EMEAAD\anchaudhary</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>Reviewer3</t>
-  </si>
-  <si>
-    <t>Reviewer2</t>
-  </si>
-  <si>
-    <t>Reviewer1</t>
-  </si>
-  <si>
-    <t>PRForm</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>STANDARD</t>
-  </si>
-  <si>
-    <t>EMEAAD\proch</t>
-  </si>
-  <si>
-    <t>Approver3</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>CP-APEX</t>
-  </si>
-  <si>
-    <t>Catering for Seminar and Events</t>
-  </si>
-  <si>
-    <t>EMEAAD\spineau</t>
-  </si>
-  <si>
-    <t>EMEAAD\msinno</t>
-  </si>
-  <si>
-    <t>S00011626001</t>
-  </si>
-  <si>
-    <t>MAD</t>
-  </si>
-  <si>
-    <t>PRSTD_119_4993_30000/2</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>Aix  Golf</t>
-  </si>
-  <si>
-    <t>4993</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
     <t>docType</t>
   </si>
   <si>
     <t>Purchase requisition</t>
+  </si>
+  <si>
+    <t>EMEAAD\ncourtin</t>
   </si>
   <si>
     <t>Test Status</t>
@@ -235,7 +223,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,26 +243,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -295,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -305,17 +281,30 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -325,18 +314,16 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
@@ -619,254 +606,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.85546875" collapsed="false"/>
     <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="17.140625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="16.140625" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
-    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="32.28515625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="31.85546875" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="29.7109375" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.7109375" collapsed="false"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="17" max="17" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="18.5703125" collapsed="false"/>
+    <col min="19" max="20" customWidth="true" width="16.140625" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="11.7109375" collapsed="false"/>
+    <col min="23" max="23" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="24" max="25" bestFit="true" customWidth="true" width="25.140625" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="27" max="16384" style="5" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="N1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="K2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" t="s" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" s="2" t="s">
+      <c r="T3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="V3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="Z3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="X2" s="10" t="s">
+      <c r="AB3" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH2" t="s" s="11">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix subcontracting and logistic Form for Prtype Text field
</commit_message>
<xml_diff>
--- a/BaswareAutomation/Output/OutputDataProvide.xlsx
+++ b/BaswareAutomation/Output/OutputDataProvide.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -324,22 +324,12 @@
   </si>
   <si>
     <t>EMEAAD\laroche</t>
-  </si>
-  <si>
-    <t>Test Status</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,32 +384,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -450,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -467,10 +437,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,41 +718,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="17.140625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="16.140625" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
-    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" customWidth="1"/>
+    <col min="19" max="19" width="26" customWidth="1"/>
+    <col min="20" max="20" width="21.85546875" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" customWidth="1"/>
+    <col min="23" max="24" width="15.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="19.7109375" customWidth="1"/>
+    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -886,9 +852,6 @@
       <c r="AF1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -987,9 +950,6 @@
       <c r="AF2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AH2" t="s" s="12">
-        <v>88</v>
-      </c>
     </row>
     <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1088,9 +1048,6 @@
       <c r="AF3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AH3" t="s" s="13">
-        <v>89</v>
-      </c>
     </row>
     <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1141,9 +1098,7 @@
       <c r="P4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="Q4" s="2"/>
       <c r="R4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1188,9 +1143,6 @@
       </c>
       <c r="AF4" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="AH4" t="s" s="14">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1289,9 +1241,6 @@
       </c>
       <c r="AF5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="AH5" t="s" s="15">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Url from Excel sheet for every Login
</commit_message>
<xml_diff>
--- a/BaswareAutomation/Output/OutputDataProvide.xlsx
+++ b/BaswareAutomation/Output/OutputDataProvide.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -324,12 +324,22 @@
   </si>
   <si>
     <t>EMEAAD\laroche</t>
+  </si>
+  <si>
+    <t>Test Status</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,12 +394,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -420,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -437,6 +467,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -718,41 +752,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" customWidth="1"/>
-    <col min="19" max="19" width="26" customWidth="1"/>
-    <col min="20" max="20" width="21.85546875" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" customWidth="1"/>
-    <col min="23" max="24" width="15.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="19.7109375" customWidth="1"/>
-    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="17.140625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" width="21.85546875" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" width="16.140625" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -852,6 +886,9 @@
       <c r="AF1" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="AH1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -950,6 +987,9 @@
       <c r="AF2" s="11" t="s">
         <v>40</v>
       </c>
+      <c r="AH2" t="s" s="12">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1048,6 +1088,9 @@
       <c r="AF3" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="AH3" t="s" s="13">
+        <v>89</v>
+      </c>
     </row>
     <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1144,6 +1187,9 @@
       <c r="AF4" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="AH4" t="s" s="14">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1241,6 +1287,9 @@
       </c>
       <c r="AF5" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="AH5" t="s" s="15">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix Select entity problem - of selecting your requisition instead of entity select
</commit_message>
<xml_diff>
--- a/BaswareAutomation/Output/OutputDataProvide.xlsx
+++ b/BaswareAutomation/Output/OutputDataProvide.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -324,22 +324,12 @@
   </si>
   <si>
     <t>EMEAAD\laroche</t>
-  </si>
-  <si>
-    <t>Test Status</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,32 +384,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -450,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -467,10 +437,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,7 +718,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -760,33 +726,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="17.140625" collapsed="false"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
-    <col min="20" max="20" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="16.140625" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
-    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" customWidth="1"/>
+    <col min="19" max="19" width="26" customWidth="1"/>
+    <col min="20" max="20" width="21.85546875" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" customWidth="1"/>
+    <col min="23" max="24" width="15.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="19.7109375" customWidth="1"/>
+    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -886,9 +852,6 @@
       <c r="AF1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -987,9 +950,6 @@
       <c r="AF2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AH2" t="s" s="12">
-        <v>88</v>
-      </c>
     </row>
     <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1088,9 +1048,6 @@
       <c r="AF3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AH3" t="s" s="13">
-        <v>89</v>
-      </c>
     </row>
     <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1187,9 +1144,6 @@
       <c r="AF4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AH4" t="s" s="14">
-        <v>89</v>
-      </c>
     </row>
     <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1287,9 +1241,6 @@
       </c>
       <c r="AF5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="AH5" t="s" s="15">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>